<commit_message>
feat[goToExcel]: add isAdmin middleware on routes post, put and delete
</commit_message>
<xml_diff>
--- a/ros.xlsx
+++ b/ros.xlsx
@@ -11,15 +11,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>celular</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>OBSERVADOR</t>
+  </si>
+  <si>
+    <t>GESTOR</t>
+  </si>
+  <si>
+    <t>ÁREA</t>
+  </si>
+  <si>
+    <t>LOCAL</t>
+  </si>
+  <si>
+    <t>NATUREZA</t>
+  </si>
+  <si>
+    <t>OPCAO</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>AÇÃO DE BLOQUEIO/ PROPOSTAS/ SUGESTOES</t>
+  </si>
+  <si>
+    <t>Parecer do Respónsável pela ação</t>
+  </si>
+  <si>
+    <t>TRATATIVAS</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>AREA RESPONSAVEL</t>
+  </si>
+  <si>
+    <t>RESPONSAVEL</t>
   </si>
   <si>
     <t>Abel</t>
@@ -29,12 +62,6 @@
   </si>
   <si>
     <t>65999010913</t>
-  </si>
-  <si>
-    <t>Marcos</t>
-  </si>
-  <si>
-    <t>marcos@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -80,13 +107,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -96,27 +123,170 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat[goToExcel]: get data to generate relactory
</commit_message>
<xml_diff>
--- a/ros.xlsx
+++ b/ros.xlsx
@@ -11,38 +11,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>DATA</t>
   </si>
   <si>
+    <t>MÊS</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
     <t>OBSERVADOR</t>
   </si>
   <si>
-    <t>GESTOR</t>
-  </si>
-  <si>
-    <t>ÁREA</t>
-  </si>
-  <si>
-    <t>LOCAL</t>
-  </si>
-  <si>
-    <t>NATUREZA</t>
-  </si>
-  <si>
-    <t>OPCAO</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO</t>
+    <t>ÁREA DA OCORRENCIA</t>
+  </si>
+  <si>
+    <t>LOCAL DA OCORRÊNCIA</t>
+  </si>
+  <si>
+    <t>REFERENTE A</t>
+  </si>
+  <si>
+    <t>OPÇÕES DE OCORRÊNCIA</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO DA OCORRÊNCIA</t>
   </si>
   <si>
     <t>AÇÃO DE BLOQUEIO/ PROPOSTAS/ SUGESTOES</t>
   </si>
   <si>
-    <t>Parecer do Respónsável pela ação</t>
-  </si>
-  <si>
     <t>TRATATIVAS</t>
   </si>
   <si>
@@ -55,13 +55,103 @@
     <t>RESPONSAVEL</t>
   </si>
   <si>
-    <t>Abel</t>
-  </si>
-  <si>
-    <t>teste@gmail.com</t>
-  </si>
-  <si>
-    <t>65999010913</t>
+    <t>23-10-2022 14:05</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Anônimo</t>
+  </si>
+  <si>
+    <t>Portaria</t>
+  </si>
+  <si>
+    <t>Planta Industrial</t>
+  </si>
+  <si>
+    <t>Segurança do Trabalho</t>
+  </si>
+  <si>
+    <t>Falta do uso do EPI</t>
+  </si>
+  <si>
+    <t>tetsteyewttae</t>
+  </si>
+  <si>
+    <t>asjdijasidjaisj</t>
+  </si>
+  <si>
+    <t>Tratado</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Jorge Leandro Nunes de Oliveira</t>
+  </si>
+  <si>
+    <t>04-10-2022 08:34</t>
+  </si>
+  <si>
+    <t>Barragem de rejeito</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
+  </si>
+  <si>
+    <t>It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
+  </si>
+  <si>
+    <t>02-10-2022 16:23</t>
+  </si>
+  <si>
+    <t>Meio Ambiente</t>
+  </si>
+  <si>
+    <t>Falta de limpeza e organização</t>
+  </si>
+  <si>
+    <t>Teste com outro responsavel</t>
+  </si>
+  <si>
+    <t>Alterar responsvel</t>
+  </si>
+  <si>
+    <t>não tratado</t>
+  </si>
+  <si>
+    <t>não resolvido</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>30-09-2022 16:15</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>Teste de envio de ROS</t>
+  </si>
+  <si>
+    <t>Teste </t>
+  </si>
+  <si>
+    <t>Não Tratado</t>
+  </si>
+  <si>
+    <t>Não Resolvido</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -107,7 +197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -168,42 +258,42 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
@@ -212,42 +302,42 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
@@ -256,37 +346,81 @@
         <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>